<commit_message>
Trình bày lại, thêm comment cho từng đoạn code.
</commit_message>
<xml_diff>
--- a/Thuyet trinh nhom 1/tonghop.xlsx
+++ b/Thuyet trinh nhom 1/tonghop.xlsx
@@ -398,7 +398,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>2460000000</v>
+        <v>25500000</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -409,7 +409,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>3030000000</v>
+        <v>33600000</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -420,7 +420,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>2670000000</v>
+        <v>27600000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>